<commit_message>
fluor design changes and spreadsheets; inw: list of tuples defining features of each subset of land. Also, deriving x-coords from given y-coords and distance between junctions
</commit_message>
<xml_diff>
--- a/dev/point375inch_pipe.xlsx
+++ b/dev/point375inch_pipe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\jamar1391.github.io\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40021EA-F6A0-477B-8FD3-CD4E63FAAF99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E75D28-1813-484C-AC83-889B8E70EFA9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2064" yWindow="1344" windowWidth="19944" windowHeight="10980" activeTab="7" xr2:uid="{F22476ED-52B1-4252-BA3D-E6827F3736A8}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="19944" windowHeight="10980" activeTab="7" xr2:uid="{F22476ED-52B1-4252-BA3D-E6827F3736A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet10" sheetId="10" r:id="rId1"/>
@@ -7442,6 +7442,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8586,8 +8587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C244507-49DC-48CB-8360-D920A51B899D}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>